<commit_message>
nearly all tracked - power and ground planes to do!
</commit_message>
<xml_diff>
--- a/HILTOP_Motherboard_BOM_Draft.xlsx
+++ b/HILTOP_Motherboard_BOM_Draft.xlsx
@@ -2461,11 +2461,12 @@
     <numFmt numFmtId="166" formatCode="0000"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2483,18 +2484,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2503,37 +2492,50 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF00864B"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2553,6 +2555,7 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2596,12 +2599,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2614,15 +2617,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2630,51 +2629,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2686,7 +2685,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2698,10 +2697,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2710,7 +2705,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Gnumeric-default" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2782,20 +2777,20 @@
   </sheetPr>
   <dimension ref="A1:M179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B133" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L173" activeCellId="0" sqref="L173"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J57" activeCellId="0" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="62.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="62.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="30.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -2891,19 +2886,19 @@
       <c r="E15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -2929,22 +2924,22 @@
       <c r="E16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="6" t="n">
+      <c r="H16" s="5" t="n">
         <v>1061</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="6" t="n">
+      <c r="J16" s="5" t="n">
         <v>1282702</v>
       </c>
-      <c r="K16" s="6" t="n">
+      <c r="K16" s="5" t="n">
         <v>1.19</v>
       </c>
       <c r="L16" s="1" t="n">
@@ -2953,37 +2948,37 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="103" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="10" t="n">
+      <c r="J17" s="9" t="n">
         <v>2581046</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="7" t="n">
         <v>0.0297</v>
       </c>
       <c r="L17" s="1" t="n">
@@ -3007,22 +3002,22 @@
       <c r="E18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="10" t="n">
+      <c r="J18" s="9" t="n">
         <v>2781412</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="7" t="n">
         <v>0.475</v>
       </c>
       <c r="L18" s="1" t="n">
@@ -3046,22 +3041,22 @@
       <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="8" t="n">
+      <c r="J19" s="7" t="n">
         <v>2611344</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="7" t="n">
         <v>0.146</v>
       </c>
       <c r="L19" s="1" t="n">
@@ -3085,22 +3080,22 @@
       <c r="E20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="8" t="n">
+      <c r="J20" s="7" t="n">
         <v>2611348</v>
       </c>
-      <c r="K20" s="8" t="n">
+      <c r="K20" s="7" t="n">
         <v>0.12</v>
       </c>
       <c r="L20" s="1" t="n">
@@ -3109,37 +3104,37 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="10" t="n">
+      <c r="J21" s="9" t="n">
         <v>2525048</v>
       </c>
-      <c r="K21" s="8" t="n">
+      <c r="K21" s="7" t="n">
         <v>0.0744</v>
       </c>
       <c r="L21" s="1" t="n">
@@ -3163,22 +3158,22 @@
       <c r="E22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="8" t="n">
+      <c r="J22" s="7" t="n">
         <v>1868426</v>
       </c>
-      <c r="K22" s="8" t="n">
+      <c r="K22" s="7" t="n">
         <v>0.459</v>
       </c>
       <c r="L22" s="1" t="n">
@@ -3202,22 +3197,22 @@
       <c r="E23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="10" t="n">
+      <c r="J23" s="9" t="n">
         <v>1327731</v>
       </c>
-      <c r="K23" s="8" t="n">
+      <c r="K23" s="7" t="n">
         <v>0.28</v>
       </c>
       <c r="L23" s="1" t="n">
@@ -3229,34 +3224,34 @@
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="10" t="n">
+      <c r="J24" s="9" t="n">
         <v>2496946</v>
       </c>
-      <c r="K24" s="8" t="n">
+      <c r="K24" s="7" t="n">
         <v>0.052</v>
       </c>
       <c r="L24" s="1" t="n">
@@ -3265,37 +3260,37 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="11" t="n">
+      <c r="B25" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="8" t="n">
+      <c r="J25" s="7" t="n">
         <v>1740572</v>
       </c>
-      <c r="K25" s="8" t="n">
+      <c r="K25" s="7" t="n">
         <v>0.133</v>
       </c>
       <c r="L25" s="1" t="n">
@@ -3307,34 +3302,34 @@
       <c r="A26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="10" t="n">
+      <c r="J26" s="9" t="n">
         <v>2496835</v>
       </c>
-      <c r="K26" s="8" t="n">
+      <c r="K26" s="7" t="n">
         <v>0.298</v>
       </c>
       <c r="L26" s="1" t="n">
@@ -3346,34 +3341,34 @@
       <c r="A27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="10" t="n">
+      <c r="J27" s="9" t="n">
         <v>1414609</v>
       </c>
-      <c r="K27" s="8" t="n">
+      <c r="K27" s="7" t="n">
         <v>0.0117</v>
       </c>
       <c r="L27" s="1" t="n">
@@ -3385,16 +3380,16 @@
       <c r="A28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B28" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>99</v>
       </c>
       <c r="L28" s="1" t="n">
@@ -3403,37 +3398,37 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="11" t="n">
+      <c r="B29" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J29" s="8" t="n">
+      <c r="J29" s="7" t="n">
         <v>1462447</v>
       </c>
-      <c r="K29" s="8" t="n">
+      <c r="K29" s="7" t="n">
         <v>0.0744</v>
       </c>
       <c r="L29" s="1" t="n">
@@ -3445,34 +3440,34 @@
       <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="11" t="n">
+      <c r="B30" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="10" t="n">
+      <c r="J30" s="9" t="n">
         <v>2118135</v>
       </c>
-      <c r="K30" s="8" t="n">
+      <c r="K30" s="7" t="n">
         <v>0.351</v>
       </c>
       <c r="L30" s="1" t="n">
@@ -3484,19 +3479,19 @@
       <c r="A31" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="11" t="n">
+      <c r="B31" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>114</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -3523,34 +3518,34 @@
       <c r="A32" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B32" s="11" t="n">
+      <c r="B32" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J32" s="8" t="n">
+      <c r="J32" s="7" t="n">
         <v>1658880</v>
       </c>
-      <c r="K32" s="8" t="n">
+      <c r="K32" s="7" t="n">
         <v>0.148</v>
       </c>
       <c r="L32" s="1" t="n">
@@ -3562,34 +3557,34 @@
       <c r="A33" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="11" t="n">
+      <c r="B33" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J33" s="10" t="n">
+      <c r="J33" s="9" t="n">
         <v>1458911</v>
       </c>
-      <c r="K33" s="8" t="n">
+      <c r="K33" s="7" t="n">
         <v>0.286</v>
       </c>
       <c r="L33" s="1" t="n">
@@ -3598,37 +3593,37 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="8" t="n">
+      <c r="J34" s="7" t="n">
         <v>1414634</v>
       </c>
-      <c r="K34" s="8" t="n">
+      <c r="K34" s="7" t="n">
         <v>0.615</v>
       </c>
       <c r="L34" s="1" t="n">
@@ -3640,34 +3635,34 @@
       <c r="A35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="11" t="n">
+      <c r="B35" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="10" t="n">
+      <c r="J35" s="9" t="n">
         <v>1658891</v>
       </c>
-      <c r="K35" s="8" t="n">
+      <c r="K35" s="7" t="n">
         <v>0.662</v>
       </c>
       <c r="L35" s="1" t="n">
@@ -3679,34 +3674,34 @@
       <c r="A36" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B36" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="11" t="s">
+      <c r="B36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J36" s="10" t="n">
+      <c r="J36" s="9" t="n">
         <v>1867963</v>
       </c>
-      <c r="K36" s="8" t="n">
+      <c r="K36" s="7" t="n">
         <v>0.384</v>
       </c>
       <c r="L36" s="1" t="n">
@@ -3718,34 +3713,34 @@
       <c r="A37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B37" s="11" t="n">
+      <c r="B37" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J37" s="8" t="n">
+      <c r="J37" s="7" t="n">
         <v>498567</v>
       </c>
-      <c r="K37" s="8" t="n">
+      <c r="K37" s="7" t="n">
         <v>0.063</v>
       </c>
       <c r="L37" s="1" t="n">
@@ -3757,34 +3752,34 @@
       <c r="A38" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="11" t="n">
+      <c r="B38" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="8" t="n">
+      <c r="J38" s="7" t="n">
         <v>2526242</v>
       </c>
-      <c r="K38" s="13" t="n">
+      <c r="K38" s="12" t="n">
         <v>0.08</v>
       </c>
       <c r="L38" s="1" t="n">
@@ -3796,34 +3791,34 @@
       <c r="A39" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B39" s="11" t="n">
+      <c r="B39" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J39" s="8" t="n">
+      <c r="J39" s="7" t="n">
         <v>316672</v>
       </c>
-      <c r="K39" s="8" t="n">
+      <c r="K39" s="7" t="n">
         <v>0.108</v>
       </c>
       <c r="L39" s="1" t="n">
@@ -3835,34 +3830,34 @@
       <c r="A40" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="11" t="n">
+      <c r="B40" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="I40" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J40" s="10" t="n">
+      <c r="J40" s="9" t="n">
         <v>2332514</v>
       </c>
-      <c r="K40" s="8" t="n">
+      <c r="K40" s="7" t="n">
         <v>0.0411</v>
       </c>
       <c r="L40" s="1" t="n">
@@ -3874,34 +3869,34 @@
       <c r="A41" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="11" t="n">
+      <c r="B41" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I41" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J41" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="K41" s="8" t="n">
+      <c r="K41" s="7" t="n">
         <v>0.31</v>
       </c>
       <c r="L41" s="1" t="n">
@@ -3913,34 +3908,34 @@
       <c r="A42" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="11" t="n">
+      <c r="B42" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G42" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J42" s="8" t="n">
+      <c r="J42" s="7" t="n">
         <v>1902422</v>
       </c>
-      <c r="K42" s="8" t="n">
+      <c r="K42" s="7" t="n">
         <v>0.086</v>
       </c>
       <c r="L42" s="1" t="n">
@@ -3964,22 +3959,22 @@
       <c r="E43" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I43" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="J43" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="K43" s="8" t="n">
+      <c r="K43" s="7" t="n">
         <v>0.43</v>
       </c>
       <c r="L43" s="1" t="n">
@@ -4003,22 +3998,22 @@
       <c r="E44" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="K44" s="8" t="n">
+      <c r="K44" s="7" t="n">
         <v>0.4</v>
       </c>
       <c r="L44" s="1" t="n">
@@ -4042,22 +4037,22 @@
       <c r="E45" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G45" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J45" s="16" t="n">
+      <c r="J45" s="15" t="n">
         <v>2317422</v>
       </c>
-      <c r="K45" s="8" t="n">
+      <c r="K45" s="7" t="n">
         <v>0.26</v>
       </c>
       <c r="L45" s="1" t="n">
@@ -4081,22 +4076,22 @@
       <c r="E46" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I46" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J46" s="8" t="n">
+      <c r="J46" s="7" t="n">
         <v>1467550</v>
       </c>
-      <c r="K46" s="8" t="n">
+      <c r="K46" s="7" t="n">
         <v>0.158</v>
       </c>
       <c r="L46" s="1" t="n">
@@ -4120,22 +4115,22 @@
       <c r="E47" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J47" s="8" t="n">
+      <c r="J47" s="7" t="n">
         <v>9556974</v>
       </c>
-      <c r="K47" s="8" t="n">
+      <c r="K47" s="7" t="n">
         <v>0.757</v>
       </c>
       <c r="L47" s="1" t="n">
@@ -4159,22 +4154,22 @@
       <c r="E48" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G48" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J48" s="8" t="n">
+      <c r="J48" s="7" t="n">
         <v>2335186</v>
       </c>
-      <c r="K48" s="8" t="n">
+      <c r="K48" s="7" t="n">
         <v>2.4</v>
       </c>
       <c r="L48" s="1" t="n">
@@ -4198,22 +4193,22 @@
       <c r="E49" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="H49" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="I49" s="6" t="s">
+      <c r="I49" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J49" s="6" t="n">
+      <c r="J49" s="5" t="n">
         <v>2509863</v>
       </c>
-      <c r="K49" s="6" t="n">
+      <c r="K49" s="5" t="n">
         <v>0.21</v>
       </c>
       <c r="L49" s="1" t="n">
@@ -4237,22 +4232,22 @@
       <c r="E50" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="H50" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="I50" s="6" t="s">
+      <c r="I50" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="J50" s="6" t="s">
+      <c r="J50" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="K50" s="6" t="n">
+      <c r="K50" s="5" t="n">
         <v>0.36</v>
       </c>
       <c r="L50" s="1" t="n">
@@ -4276,22 +4271,22 @@
       <c r="E51" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="I51" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J51" s="8" t="n">
+      <c r="J51" s="7" t="n">
         <v>1467550</v>
       </c>
-      <c r="K51" s="8" t="n">
+      <c r="K51" s="7" t="n">
         <v>0.158</v>
       </c>
       <c r="L51" s="1" t="n">
@@ -4315,22 +4310,22 @@
       <c r="E52" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="G52" s="5" t="s">
+      <c r="G52" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="I52" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J52" s="5" t="n">
+      <c r="J52" s="4" t="n">
         <v>2215314</v>
       </c>
-      <c r="K52" s="5" t="n">
+      <c r="K52" s="4" t="n">
         <v>0.521</v>
       </c>
       <c r="L52" s="1" t="n">
@@ -4354,22 +4349,22 @@
       <c r="E53" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="H53" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="I53" s="6" t="s">
+      <c r="I53" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J53" s="6" t="n">
+      <c r="J53" s="5" t="n">
         <v>2810350</v>
       </c>
-      <c r="K53" s="6" t="n">
+      <c r="K53" s="5" t="n">
         <v>0.611</v>
       </c>
       <c r="L53" s="1" t="n">
@@ -4393,22 +4388,22 @@
       <c r="E54" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F54" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G54" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="H54" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="I54" s="6" t="s">
+      <c r="I54" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J54" s="6" t="n">
+      <c r="J54" s="5" t="n">
         <v>2752736</v>
       </c>
-      <c r="K54" s="6" t="n">
+      <c r="K54" s="5" t="n">
         <v>0.367</v>
       </c>
       <c r="L54" s="1" t="n">
@@ -4432,22 +4427,22 @@
       <c r="E55" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G55" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I55" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J55" s="8" t="n">
+      <c r="J55" s="7" t="n">
         <v>1515672</v>
       </c>
-      <c r="K55" s="8" t="n">
+      <c r="K55" s="7" t="n">
         <v>0.0415</v>
       </c>
       <c r="L55" s="1" t="n">
@@ -4471,22 +4466,22 @@
       <c r="E56" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="H56" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="I56" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J56" s="16" t="s">
+      <c r="J56" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="K56" s="8" t="n">
+      <c r="K56" s="7" t="n">
         <v>0.73</v>
       </c>
       <c r="L56" s="1" t="n">
@@ -4510,22 +4505,22 @@
       <c r="E57" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G57" s="5" t="s">
+      <c r="G57" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="I57" s="5" t="s">
+      <c r="I57" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="J57" s="5" t="s">
+      <c r="J57" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="K57" s="5" t="n">
+      <c r="K57" s="4" t="n">
         <v>0.57</v>
       </c>
       <c r="L57" s="1" t="n">
@@ -4549,22 +4544,22 @@
       <c r="E58" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G58" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H58" s="18" t="s">
+      <c r="H58" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="I58" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J58" s="6" t="n">
+      <c r="J58" s="5" t="n">
         <v>9731679</v>
       </c>
-      <c r="K58" s="5" t="n">
+      <c r="K58" s="4" t="n">
         <v>0.251</v>
       </c>
       <c r="L58" s="1" t="n">
@@ -4588,22 +4583,22 @@
       <c r="E59" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G59" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J59" s="5" t="s">
+      <c r="J59" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="K59" s="5" t="n">
+      <c r="K59" s="4" t="n">
         <v>0.99</v>
       </c>
       <c r="L59" s="1" t="n">
@@ -4627,22 +4622,22 @@
       <c r="E60" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G60" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="I60" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="J60" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="K60" s="5" t="n">
+      <c r="K60" s="4" t="n">
         <v>0.33</v>
       </c>
       <c r="L60" s="1" t="n">
@@ -4666,22 +4661,22 @@
       <c r="E61" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="G61" s="5" t="s">
+      <c r="G61" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J61" s="18" t="s">
+      <c r="J61" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="K61" s="5" t="n">
+      <c r="K61" s="4" t="n">
         <v>0.02</v>
       </c>
       <c r="L61" s="1" t="n">
@@ -4705,22 +4700,22 @@
       <c r="E62" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="G62" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J62" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="K62" s="5" t="n">
+      <c r="K62" s="4" t="n">
         <v>0.02</v>
       </c>
       <c r="L62" s="1" t="n">
@@ -4744,22 +4739,22 @@
       <c r="E63" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="G63" s="5" t="s">
+      <c r="G63" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H63" s="18" t="s">
+      <c r="H63" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J63" s="18" t="s">
+      <c r="J63" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="K63" s="5" t="n">
+      <c r="K63" s="4" t="n">
         <v>1.08</v>
       </c>
       <c r="L63" s="1" t="n">
@@ -4783,22 +4778,22 @@
       <c r="E64" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="G64" s="5" t="s">
+      <c r="G64" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J64" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="K64" s="5" t="n">
+      <c r="K64" s="4" t="n">
         <v>0.32</v>
       </c>
       <c r="L64" s="1" t="n">
@@ -4822,22 +4817,22 @@
       <c r="E65" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G65" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J65" s="5" t="s">
+      <c r="J65" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="K65" s="5" t="n">
+      <c r="K65" s="4" t="n">
         <v>0.32</v>
       </c>
       <c r="L65" s="1" t="n">
@@ -4861,22 +4856,22 @@
       <c r="E66" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G66" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I66" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J66" s="5" t="s">
+      <c r="J66" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="K66" s="5" t="n">
+      <c r="K66" s="4" t="n">
         <v>1.26</v>
       </c>
       <c r="L66" s="1" t="n">
@@ -4900,22 +4895,22 @@
       <c r="E67" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="G67" s="5" t="s">
+      <c r="G67" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I67" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J67" s="5" t="n">
+      <c r="J67" s="4" t="n">
         <v>1572191</v>
       </c>
-      <c r="K67" s="5" t="n">
+      <c r="K67" s="4" t="n">
         <v>4.38</v>
       </c>
       <c r="L67" s="1" t="n">
@@ -4939,22 +4934,22 @@
       <c r="E68" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G68" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J68" s="5" t="n">
+      <c r="J68" s="4" t="n">
         <v>1519801</v>
       </c>
-      <c r="K68" s="5" t="n">
+      <c r="K68" s="4" t="n">
         <v>0.584</v>
       </c>
       <c r="L68" s="1" t="n">
@@ -4978,22 +4973,22 @@
       <c r="E69" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G69" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J69" s="5" t="n">
+      <c r="J69" s="4" t="n">
         <v>9731164</v>
       </c>
-      <c r="K69" s="5" t="n">
+      <c r="K69" s="4" t="n">
         <v>0.232</v>
       </c>
       <c r="L69" s="1" t="n">
@@ -5017,22 +5012,22 @@
       <c r="E70" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="G70" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J70" s="5" t="n">
+      <c r="J70" s="4" t="n">
         <v>673237</v>
       </c>
-      <c r="K70" s="5" t="n">
+      <c r="K70" s="4" t="n">
         <v>0.238</v>
       </c>
       <c r="L70" s="1" t="n">
@@ -5056,22 +5051,22 @@
       <c r="E71" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G71" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J71" s="18" t="n">
+      <c r="J71" s="17" t="n">
         <v>673262</v>
       </c>
-      <c r="K71" s="5" t="n">
+      <c r="K71" s="4" t="n">
         <v>0.501</v>
       </c>
       <c r="L71" s="1" t="n">
@@ -5095,22 +5090,22 @@
       <c r="E72" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="G72" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="I72" s="5" t="s">
+      <c r="I72" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J72" s="18" t="n">
+      <c r="J72" s="17" t="n">
         <v>673249</v>
       </c>
-      <c r="K72" s="5" t="n">
+      <c r="K72" s="4" t="n">
         <v>0.314</v>
       </c>
       <c r="L72" s="1" t="n">
@@ -5134,22 +5129,22 @@
       <c r="E73" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="G73" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J73" s="6" t="n">
+      <c r="J73" s="5" t="n">
         <v>9731156</v>
       </c>
-      <c r="K73" s="5" t="n">
+      <c r="K73" s="4" t="n">
         <v>0.184</v>
       </c>
       <c r="L73" s="1" t="n">
@@ -5173,22 +5168,22 @@
       <c r="E74" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="G74" s="5" t="s">
+      <c r="G74" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="I74" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J74" s="5" t="s">
+      <c r="J74" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="K74" s="5" t="n">
+      <c r="K74" s="4" t="n">
         <v>0.33</v>
       </c>
       <c r="L74" s="1" t="n">
@@ -5212,22 +5207,22 @@
       <c r="E75" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="G75" s="5" t="s">
+      <c r="G75" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="H75" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J75" s="18" t="s">
+      <c r="J75" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="K75" s="5" t="n">
+      <c r="K75" s="4" t="n">
         <v>0.45</v>
       </c>
       <c r="L75" s="1" t="n">
@@ -5251,22 +5246,22 @@
       <c r="E76" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="G76" s="5" t="s">
+      <c r="G76" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H76" s="18" t="s">
+      <c r="H76" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="I76" s="5" t="s">
+      <c r="I76" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J76" s="18" t="s">
+      <c r="J76" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="K76" s="5" t="n">
+      <c r="K76" s="4" t="n">
         <v>0.32</v>
       </c>
       <c r="L76" s="1" t="n">
@@ -5290,22 +5285,22 @@
       <c r="E77" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="G77" s="5" t="s">
+      <c r="G77" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J77" s="5" t="s">
+      <c r="J77" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="K77" s="5" t="n">
+      <c r="K77" s="4" t="n">
         <v>0.52</v>
       </c>
       <c r="L77" s="1" t="n">
@@ -5329,22 +5324,22 @@
       <c r="E78" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="G78" s="5" t="s">
+      <c r="G78" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J78" s="5" t="n">
+      <c r="J78" s="4" t="n">
         <v>2215306</v>
       </c>
-      <c r="K78" s="5" t="n">
+      <c r="K78" s="4" t="n">
         <v>0.29</v>
       </c>
       <c r="L78" s="1" t="n">
@@ -5368,22 +5363,22 @@
       <c r="E79" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="G79" s="5" t="s">
+      <c r="G79" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="H79" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="I79" s="5" t="s">
+      <c r="I79" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J79" s="5" t="n">
+      <c r="J79" s="4" t="n">
         <v>2112525</v>
       </c>
-      <c r="K79" s="5" t="n">
+      <c r="K79" s="4" t="n">
         <v>2.76</v>
       </c>
       <c r="L79" s="1" t="n">
@@ -5407,22 +5402,22 @@
       <c r="E80" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="G80" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H80" s="18" t="s">
+      <c r="H80" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="I80" s="5" t="s">
+      <c r="I80" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J80" s="18" t="s">
+      <c r="J80" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="K80" s="5" t="n">
+      <c r="K80" s="4" t="n">
         <v>0.04</v>
       </c>
       <c r="L80" s="1" t="n">
@@ -5446,22 +5441,22 @@
       <c r="E81" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="G81" s="5" t="s">
+      <c r="G81" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="H81" s="4" t="s">
         <v>409</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="J81" s="5" t="s">
+      <c r="J81" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="K81" s="5" t="n">
+      <c r="K81" s="4" t="n">
         <v>0.548</v>
       </c>
       <c r="L81" s="1" t="n">
@@ -5485,22 +5480,22 @@
       <c r="E82" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="F82" s="19" t="s">
+      <c r="F82" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="G82" s="20" t="s">
+      <c r="G82" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H82" s="21" t="s">
+      <c r="H82" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="I82" s="8" t="s">
+      <c r="I82" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J82" s="6" t="n">
+      <c r="J82" s="5" t="n">
         <v>2345218</v>
       </c>
-      <c r="K82" s="8" t="n">
+      <c r="K82" s="7" t="n">
         <v>0.35</v>
       </c>
       <c r="L82" s="1" t="n">
@@ -5524,22 +5519,22 @@
       <c r="E83" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="F83" s="19" t="s">
+      <c r="F83" s="18" t="s">
         <v>421</v>
       </c>
-      <c r="G83" s="20" t="s">
+      <c r="G83" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H83" s="21" t="s">
+      <c r="H83" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="I83" s="8" t="s">
+      <c r="I83" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="J83" s="6" t="s">
+      <c r="J83" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="K83" s="8" t="n">
+      <c r="K83" s="7" t="n">
         <v>0.478</v>
       </c>
       <c r="L83" s="1" t="n">
@@ -5563,22 +5558,22 @@
       <c r="E84" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="F84" s="19" t="s">
+      <c r="F84" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="G84" s="20" t="s">
+      <c r="G84" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H84" s="21" t="s">
+      <c r="H84" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="I84" s="8" t="s">
+      <c r="I84" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J84" s="6" t="n">
+      <c r="J84" s="5" t="n">
         <v>2345220</v>
       </c>
-      <c r="K84" s="8" t="n">
+      <c r="K84" s="7" t="n">
         <v>0.509</v>
       </c>
       <c r="L84" s="1" t="n">
@@ -5602,22 +5597,22 @@
       <c r="E85" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="F85" s="19" t="s">
+      <c r="F85" s="18" t="s">
         <v>434</v>
       </c>
-      <c r="G85" s="20" t="s">
+      <c r="G85" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="H85" s="21" t="s">
+      <c r="H85" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="I85" s="8" t="s">
+      <c r="I85" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="J85" s="21" t="s">
+      <c r="J85" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="K85" s="8" t="n">
+      <c r="K85" s="7" t="n">
         <v>3.22</v>
       </c>
       <c r="L85" s="1" t="n">
@@ -5644,22 +5639,22 @@
       <c r="E86" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F86" s="19" t="s">
+      <c r="F86" s="18" t="s">
         <v>441</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H86" s="21" t="s">
+      <c r="H86" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="I86" s="8" t="s">
+      <c r="I86" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="J86" s="6" t="s">
+      <c r="J86" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="K86" s="8" t="n">
+      <c r="K86" s="7" t="n">
         <v>0.26</v>
       </c>
       <c r="L86" s="1" t="n">
@@ -5683,22 +5678,22 @@
       <c r="E87" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="F87" s="6" t="s">
+      <c r="F87" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="G87" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="H87" s="6" t="s">
+      <c r="H87" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="I87" s="6" t="s">
+      <c r="I87" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J87" s="6" t="n">
+      <c r="J87" s="5" t="n">
         <v>1510761</v>
       </c>
-      <c r="K87" s="6" t="n">
+      <c r="K87" s="5" t="n">
         <v>0.097</v>
       </c>
       <c r="L87" s="1" t="n">
@@ -5722,22 +5717,22 @@
       <c r="E88" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F88" s="6" t="s">
+      <c r="F88" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="G88" s="9" t="s">
+      <c r="G88" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="H88" s="6" t="s">
+      <c r="H88" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="I88" s="6" t="s">
+      <c r="I88" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="J88" s="6" t="s">
+      <c r="J88" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="K88" s="6" t="n">
+      <c r="K88" s="5" t="n">
         <v>1.45</v>
       </c>
       <c r="L88" s="1" t="n">
@@ -5761,22 +5756,22 @@
       <c r="E89" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="F89" s="6" t="s">
+      <c r="F89" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="G89" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="H89" s="6" t="s">
+      <c r="H89" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="I89" s="6" t="s">
+      <c r="I89" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J89" s="6" t="n">
+      <c r="J89" s="5" t="n">
         <v>9525769</v>
       </c>
-      <c r="K89" s="6" t="n">
+      <c r="K89" s="5" t="n">
         <v>0.397</v>
       </c>
       <c r="L89" s="1" t="n">
@@ -5800,22 +5795,22 @@
       <c r="E90" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="F90" s="6" t="s">
+      <c r="F90" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="G90" s="9" t="s">
+      <c r="G90" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="H90" s="6" t="s">
+      <c r="H90" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="I90" s="6" t="s">
+      <c r="I90" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="J90" s="15" t="s">
+      <c r="J90" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="K90" s="6" t="n">
+      <c r="K90" s="5" t="n">
         <v>0.41</v>
       </c>
       <c r="L90" s="1" t="n">
@@ -5824,22 +5819,22 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="B91" s="7" t="n">
+      <c r="B91" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="D91" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E91" s="7" t="s">
+      <c r="E91" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="F91" s="22" t="s">
+      <c r="F91" s="20" t="s">
         <v>469</v>
       </c>
       <c r="L91" s="1" t="n">
@@ -5848,19 +5843,19 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="B92" s="7" t="n">
+      <c r="B92" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E92" s="7" t="s">
+      <c r="E92" s="6" t="s">
         <v>472</v>
       </c>
       <c r="L92" s="1" t="n">
@@ -5890,19 +5885,19 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="B94" s="7" t="n">
+      <c r="B94" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E94" s="7" t="s">
+      <c r="E94" s="6" t="s">
         <v>476</v>
       </c>
       <c r="L94" s="1" t="n">
@@ -5932,19 +5927,19 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="B96" s="7" t="n">
+      <c r="B96" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C96" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E96" s="7" t="s">
+      <c r="E96" s="6" t="s">
         <v>481</v>
       </c>
       <c r="L96" s="1" t="n">
@@ -5953,19 +5948,19 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B97" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C97" s="7" t="s">
+      <c r="B97" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E97" s="7" t="s">
+      <c r="E97" s="6" t="s">
         <v>484</v>
       </c>
       <c r="L97" s="1" t="n">
@@ -5974,19 +5969,19 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="B98" s="7" t="n">
+      <c r="B98" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D98" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E98" s="7" t="s">
+      <c r="E98" s="6" t="s">
         <v>487</v>
       </c>
       <c r="L98" s="1" t="n">
@@ -5995,19 +5990,19 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="s">
+      <c r="A99" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="B99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C99" s="7" t="s">
+      <c r="B99" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D99" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E99" s="7" t="s">
+      <c r="E99" s="6" t="s">
         <v>490</v>
       </c>
       <c r="L99" s="1" t="n">
@@ -6016,19 +6011,19 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="s">
+      <c r="A100" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="B100" s="7" t="n">
+      <c r="B100" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="D100" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E100" s="7" t="s">
+      <c r="E100" s="6" t="s">
         <v>493</v>
       </c>
       <c r="L100" s="1" t="n">
@@ -6037,19 +6032,19 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="B101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C101" s="7" t="s">
+      <c r="B101" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="E101" s="7" t="s">
+      <c r="E101" s="6" t="s">
         <v>496</v>
       </c>
       <c r="L101" s="1" t="n">
@@ -6079,19 +6074,19 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="7" t="s">
+      <c r="A103" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="B103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C103" s="7" t="s">
+      <c r="B103" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D103" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="E103" s="7" t="s">
+      <c r="E103" s="6" t="s">
         <v>500</v>
       </c>
       <c r="L103" s="1" t="n">
@@ -6100,19 +6095,19 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="7" t="s">
+      <c r="A104" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="B104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C104" s="7" t="s">
+      <c r="B104" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D104" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E104" s="7" t="s">
+      <c r="E104" s="6" t="s">
         <v>503</v>
       </c>
       <c r="L104" s="1" t="n">
@@ -6121,19 +6116,19 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="B105" s="7" t="n">
+      <c r="B105" s="6" t="n">
         <v>32</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D105" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="E105" s="7" t="s">
+      <c r="E105" s="6" t="s">
         <v>507</v>
       </c>
       <c r="L105" s="1" t="n">
@@ -6142,19 +6137,19 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="7" t="s">
+      <c r="A106" s="6" t="s">
         <v>508</v>
       </c>
-      <c r="B106" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C106" s="7" t="s">
+      <c r="B106" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" s="6" t="s">
         <v>509</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="D106" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E106" s="7" t="s">
+      <c r="E106" s="6" t="s">
         <v>510</v>
       </c>
       <c r="L106" s="1" t="n">
@@ -6163,19 +6158,19 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="B107" s="7" t="n">
+      <c r="B107" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="D107" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E107" s="7" t="s">
+      <c r="E107" s="6" t="s">
         <v>513</v>
       </c>
       <c r="L107" s="1" t="n">
@@ -6184,19 +6179,19 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="B108" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C108" s="7" t="s">
+      <c r="B108" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="D108" s="7" t="s">
+      <c r="D108" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E108" s="7" t="s">
+      <c r="E108" s="6" t="s">
         <v>516</v>
       </c>
       <c r="L108" s="1" t="n">
@@ -6205,19 +6200,19 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="B109" s="7" t="n">
+      <c r="B109" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C109" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="D109" s="7" t="s">
+      <c r="D109" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="E109" s="7" t="s">
+      <c r="E109" s="6" t="s">
         <v>518</v>
       </c>
       <c r="L109" s="1" t="n">
@@ -6247,19 +6242,19 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="B111" s="7" t="n">
+      <c r="B111" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C111" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="D111" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="E111" s="7" t="s">
+      <c r="E111" s="6" t="s">
         <v>521</v>
       </c>
       <c r="L111" s="1" t="n">
@@ -6268,19 +6263,19 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="B112" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C112" s="7" t="s">
+      <c r="B112" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C112" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D112" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E112" s="7" t="s">
+      <c r="E112" s="6" t="s">
         <v>524</v>
       </c>
       <c r="L112" s="1" t="n">
@@ -6289,19 +6284,19 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="B113" s="7" t="n">
+      <c r="B113" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C113" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D113" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E113" s="7" t="s">
+      <c r="E113" s="6" t="s">
         <v>527</v>
       </c>
       <c r="L113" s="1" t="n">
@@ -6310,19 +6305,19 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="B114" s="7" t="n">
+      <c r="B114" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C114" s="6" t="s">
         <v>509</v>
       </c>
-      <c r="D114" s="7" t="s">
+      <c r="D114" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="E114" s="7" t="s">
+      <c r="E114" s="6" t="s">
         <v>529</v>
       </c>
       <c r="L114" s="1" t="n">
@@ -6331,19 +6326,19 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B115" s="7" t="n">
+      <c r="B115" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C115" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="D115" s="7" t="s">
+      <c r="D115" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E115" s="7" t="s">
+      <c r="E115" s="6" t="s">
         <v>532</v>
       </c>
       <c r="L115" s="1" t="n">
@@ -6352,19 +6347,19 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="B116" s="7" t="n">
+      <c r="B116" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="D116" s="7" t="s">
+      <c r="D116" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="E116" s="7" t="s">
+      <c r="E116" s="6" t="s">
         <v>535</v>
       </c>
       <c r="L116" s="1" t="n">
@@ -6373,19 +6368,19 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="7" t="s">
+      <c r="A117" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="B117" s="7" t="n">
+      <c r="B117" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="C117" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="D117" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E117" s="7" t="s">
+      <c r="E117" s="6" t="s">
         <v>538</v>
       </c>
       <c r="L117" s="1" t="n">
@@ -6394,19 +6389,19 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="B118" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C118" s="7" t="s">
+      <c r="B118" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="D118" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E118" s="7" t="s">
+      <c r="E118" s="6" t="s">
         <v>541</v>
       </c>
       <c r="L118" s="1" t="n">
@@ -6415,19 +6410,19 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="B119" s="7" t="n">
+      <c r="B119" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="D119" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E119" s="7" t="s">
+      <c r="E119" s="6" t="s">
         <v>544</v>
       </c>
       <c r="L119" s="1" t="n">
@@ -6436,19 +6431,19 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="7" t="s">
+      <c r="A120" s="6" t="s">
         <v>545</v>
       </c>
-      <c r="B120" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C120" s="7" t="s">
+      <c r="B120" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="D120" s="7" t="s">
+      <c r="D120" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E120" s="7" t="s">
+      <c r="E120" s="6" t="s">
         <v>547</v>
       </c>
       <c r="L120" s="1" t="n">
@@ -6457,19 +6452,19 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="7" t="s">
+      <c r="A121" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="B121" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C121" s="7" t="s">
+      <c r="B121" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="D121" s="7" t="s">
+      <c r="D121" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="E121" s="7" t="s">
+      <c r="E121" s="6" t="s">
         <v>549</v>
       </c>
       <c r="L121" s="1" t="n">
@@ -6478,19 +6473,19 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="7" t="s">
+      <c r="A122" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="B122" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C122" s="7" t="s">
+      <c r="B122" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="D122" s="7" t="s">
+      <c r="D122" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E122" s="7" t="s">
+      <c r="E122" s="6" t="s">
         <v>552</v>
       </c>
       <c r="L122" s="1" t="n">
@@ -6499,19 +6494,19 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="7" t="s">
+      <c r="A123" s="6" t="s">
         <v>553</v>
       </c>
-      <c r="B123" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C123" s="7" t="s">
+      <c r="B123" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" s="6" t="s">
         <v>554</v>
       </c>
-      <c r="D123" s="7" t="s">
+      <c r="D123" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E123" s="7" t="s">
+      <c r="E123" s="6" t="s">
         <v>555</v>
       </c>
       <c r="L123" s="1" t="n">
@@ -6520,19 +6515,19 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="7" t="s">
+      <c r="A124" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="B124" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C124" s="7" t="s">
+      <c r="B124" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D124" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E124" s="7" t="s">
+      <c r="E124" s="6" t="s">
         <v>558</v>
       </c>
       <c r="L124" s="1" t="n">
@@ -6556,22 +6551,22 @@
       <c r="E125" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="F125" s="8" t="s">
+      <c r="F125" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="G125" s="9" t="s">
+      <c r="G125" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="H125" s="8" t="s">
+      <c r="H125" s="7" t="s">
         <v>564</v>
       </c>
-      <c r="I125" s="8" t="s">
+      <c r="I125" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J125" s="8" t="s">
+      <c r="J125" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="K125" s="8" t="n">
+      <c r="K125" s="7" t="n">
         <v>0.66</v>
       </c>
       <c r="L125" s="1" t="n">
@@ -6580,19 +6575,19 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="7" t="s">
+      <c r="A126" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="B126" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C126" s="7" t="s">
+      <c r="B126" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C126" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="D126" s="7" t="s">
+      <c r="D126" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E126" s="7" t="s">
+      <c r="E126" s="6" t="s">
         <v>568</v>
       </c>
       <c r="L126" s="1" t="n">
@@ -6601,19 +6596,19 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="B127" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C127" s="7" t="s">
+      <c r="B127" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" s="6" t="s">
         <v>570</v>
       </c>
-      <c r="D127" s="7" t="s">
+      <c r="D127" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E127" s="7" t="s">
+      <c r="E127" s="6" t="s">
         <v>571</v>
       </c>
       <c r="L127" s="1" t="n">
@@ -6622,19 +6617,19 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="7" t="s">
+      <c r="A128" s="6" t="s">
         <v>572</v>
       </c>
-      <c r="B128" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C128" s="7" t="s">
+      <c r="B128" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" s="6" t="s">
         <v>573</v>
       </c>
-      <c r="D128" s="7" t="s">
+      <c r="D128" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E128" s="7" t="s">
+      <c r="E128" s="6" t="s">
         <v>574</v>
       </c>
       <c r="L128" s="1" t="n">
@@ -6643,19 +6638,19 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="7" t="s">
+      <c r="A129" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="B129" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C129" s="7" t="s">
+      <c r="B129" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C129" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="D129" s="7" t="s">
+      <c r="D129" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E129" s="7" t="s">
+      <c r="E129" s="6" t="s">
         <v>577</v>
       </c>
       <c r="L129" s="1" t="n">
@@ -6664,19 +6659,19 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="7" t="s">
+      <c r="A130" s="6" t="s">
         <v>578</v>
       </c>
-      <c r="B130" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C130" s="7" t="s">
+      <c r="B130" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>579</v>
       </c>
-      <c r="D130" s="7" t="s">
+      <c r="D130" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E130" s="7" t="s">
+      <c r="E130" s="6" t="s">
         <v>580</v>
       </c>
       <c r="L130" s="1" t="n">
@@ -6685,19 +6680,19 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="7" t="s">
+      <c r="A131" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="B131" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C131" s="7" t="s">
+      <c r="B131" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="D131" s="7" t="s">
+      <c r="D131" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E131" s="7" t="s">
+      <c r="E131" s="6" t="s">
         <v>468</v>
       </c>
       <c r="L131" s="1" t="n">
@@ -6742,22 +6737,22 @@
       <c r="E133" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="F133" s="6" t="s">
+      <c r="F133" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="G133" s="9" t="s">
+      <c r="G133" s="8" t="s">
         <v>589</v>
       </c>
-      <c r="H133" s="8" t="s">
+      <c r="H133" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="I133" s="6" t="s">
+      <c r="I133" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J133" s="6" t="n">
+      <c r="J133" s="5" t="n">
         <v>9659331</v>
       </c>
-      <c r="K133" s="6" t="n">
+      <c r="K133" s="5" t="n">
         <v>0.715</v>
       </c>
       <c r="L133" s="1" t="n">
@@ -6802,22 +6797,22 @@
       <c r="E135" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="F135" s="8" t="s">
+      <c r="F135" s="7" t="s">
         <v>598</v>
       </c>
-      <c r="G135" s="9" t="s">
+      <c r="G135" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="H135" s="8" t="s">
+      <c r="H135" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="I135" s="8" t="s">
+      <c r="I135" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="J135" s="8" t="s">
+      <c r="J135" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="K135" s="8" t="n">
+      <c r="K135" s="7" t="n">
         <v>0.681</v>
       </c>
       <c r="L135" s="1" t="n">
@@ -6841,22 +6836,22 @@
       <c r="E136" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="F136" s="6" t="s">
+      <c r="F136" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="G136" s="9" t="s">
+      <c r="G136" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="H136" s="6" t="s">
+      <c r="H136" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="I136" s="6" t="s">
+      <c r="I136" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J136" s="6" t="n">
+      <c r="J136" s="5" t="n">
         <v>9665005</v>
       </c>
-      <c r="K136" s="6" t="n">
+      <c r="K136" s="5" t="n">
         <v>0.926</v>
       </c>
       <c r="L136" s="1" t="n">
@@ -6880,22 +6875,22 @@
       <c r="E137" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="F137" s="8" t="s">
+      <c r="F137" s="7" t="s">
         <v>611</v>
       </c>
-      <c r="G137" s="9" t="s">
+      <c r="G137" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H137" s="8" t="s">
+      <c r="H137" s="7" t="s">
         <v>608</v>
       </c>
-      <c r="I137" s="8" t="s">
+      <c r="I137" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J137" s="8" t="s">
+      <c r="J137" s="7" t="s">
         <v>612</v>
       </c>
-      <c r="K137" s="8" t="n">
+      <c r="K137" s="7" t="n">
         <v>0.979</v>
       </c>
       <c r="L137" s="1" t="n">
@@ -6919,22 +6914,22 @@
       <c r="E138" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="F138" s="8" t="s">
+      <c r="F138" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="G138" s="9" t="s">
+      <c r="G138" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H138" s="8" t="s">
+      <c r="H138" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="I138" s="8" t="s">
+      <c r="I138" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J138" s="8" t="n">
+      <c r="J138" s="7" t="n">
         <v>2292607</v>
       </c>
-      <c r="K138" s="8" t="n">
+      <c r="K138" s="7" t="n">
         <v>3.16</v>
       </c>
       <c r="L138" s="1" t="n">
@@ -6958,22 +6953,22 @@
       <c r="E139" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="F139" s="6" t="s">
+      <c r="F139" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="G139" s="9" t="s">
+      <c r="G139" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H139" s="6" t="s">
+      <c r="H139" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="I139" s="6" t="s">
+      <c r="I139" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J139" s="6" t="n">
+      <c r="J139" s="5" t="n">
         <v>2509898</v>
       </c>
-      <c r="K139" s="6" t="n">
+      <c r="K139" s="5" t="n">
         <v>0.7</v>
       </c>
       <c r="L139" s="1" t="n">
@@ -6997,22 +6992,22 @@
       <c r="E140" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="F140" s="6" t="s">
+      <c r="F140" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="G140" s="9" t="s">
+      <c r="G140" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="H140" s="6" t="s">
+      <c r="H140" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="I140" s="6" t="s">
+      <c r="I140" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J140" s="6" t="n">
+      <c r="J140" s="5" t="n">
         <v>1827640</v>
       </c>
-      <c r="K140" s="6" t="n">
+      <c r="K140" s="5" t="n">
         <v>0.685</v>
       </c>
       <c r="L140" s="1" t="n">
@@ -7036,22 +7031,22 @@
       <c r="E141" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="F141" s="8" t="s">
+      <c r="F141" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="G141" s="9" t="s">
+      <c r="G141" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H141" s="8" t="s">
+      <c r="H141" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="I141" s="8" t="s">
+      <c r="I141" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="J141" s="8" t="s">
+      <c r="J141" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="K141" s="8" t="n">
+      <c r="K141" s="7" t="n">
         <v>4.285</v>
       </c>
       <c r="L141" s="1" t="n">
@@ -7075,22 +7070,22 @@
       <c r="E142" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="F142" s="8" t="s">
+      <c r="F142" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="G142" s="9" t="s">
+      <c r="G142" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H142" s="8" t="s">
+      <c r="H142" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="I142" s="8" t="s">
+      <c r="I142" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="J142" s="8" t="s">
+      <c r="J142" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="K142" s="8" t="n">
+      <c r="K142" s="7" t="n">
         <v>0.206</v>
       </c>
       <c r="L142" s="1" t="n">
@@ -7114,22 +7109,22 @@
       <c r="E143" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="F143" s="8" t="s">
+      <c r="F143" s="7" t="s">
         <v>647</v>
       </c>
-      <c r="G143" s="9" t="s">
+      <c r="G143" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H143" s="8" t="s">
+      <c r="H143" s="7" t="s">
         <v>644</v>
       </c>
-      <c r="I143" s="8" t="s">
+      <c r="I143" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="J143" s="8" t="s">
+      <c r="J143" s="7" t="s">
         <v>649</v>
       </c>
-      <c r="K143" s="8" t="n">
+      <c r="K143" s="7" t="n">
         <v>1.08</v>
       </c>
       <c r="L143" s="1" t="n">
@@ -7153,22 +7148,22 @@
       <c r="E144" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="F144" s="8" t="s">
+      <c r="F144" s="7" t="s">
         <v>653</v>
       </c>
-      <c r="G144" s="9" t="s">
+      <c r="G144" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H144" s="8" t="s">
+      <c r="H144" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="I144" s="8" t="s">
+      <c r="I144" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J144" s="8" t="n">
+      <c r="J144" s="7" t="n">
         <v>1754773</v>
       </c>
-      <c r="K144" s="8" t="n">
+      <c r="K144" s="7" t="n">
         <v>1.19</v>
       </c>
       <c r="L144" s="1" t="n">
@@ -7192,22 +7187,22 @@
       <c r="E145" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="F145" s="6" t="s">
+      <c r="F145" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="G145" s="9" t="s">
+      <c r="G145" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="H145" s="6" t="s">
+      <c r="H145" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="I145" s="6" t="s">
+      <c r="I145" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J145" s="6" t="n">
+      <c r="J145" s="5" t="n">
         <v>1854077</v>
       </c>
-      <c r="K145" s="6" t="n">
+      <c r="K145" s="5" t="n">
         <v>0.385</v>
       </c>
       <c r="L145" s="1" t="n">
@@ -7231,22 +7226,22 @@
       <c r="E146" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="F146" s="8" t="s">
+      <c r="F146" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="G146" s="9" t="s">
+      <c r="G146" s="8" t="s">
         <v>665</v>
       </c>
-      <c r="H146" s="8" t="s">
+      <c r="H146" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="I146" s="8" t="s">
+      <c r="I146" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J146" s="8" t="n">
+      <c r="J146" s="7" t="n">
         <v>2515822</v>
       </c>
-      <c r="K146" s="8" t="n">
+      <c r="K146" s="7" t="n">
         <v>1.85</v>
       </c>
       <c r="L146" s="1" t="n">
@@ -7270,22 +7265,22 @@
       <c r="E147" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="F147" s="6" t="s">
+      <c r="F147" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="G147" s="9" t="s">
+      <c r="G147" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H147" s="6" t="s">
+      <c r="H147" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="I147" s="6" t="s">
+      <c r="I147" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J147" s="6" t="n">
+      <c r="J147" s="5" t="n">
         <v>2492273</v>
       </c>
-      <c r="K147" s="6" t="n">
+      <c r="K147" s="5" t="n">
         <v>0.496</v>
       </c>
       <c r="L147" s="1" t="n">
@@ -7309,22 +7304,22 @@
       <c r="E148" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="F148" s="6" t="s">
+      <c r="F148" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="G148" s="9" t="s">
+      <c r="G148" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H148" s="15" t="s">
+      <c r="H148" s="14" t="s">
         <v>673</v>
       </c>
-      <c r="I148" s="6" t="s">
+      <c r="I148" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J148" s="6" t="n">
+      <c r="J148" s="5" t="n">
         <v>2211340</v>
       </c>
-      <c r="K148" s="6" t="n">
+      <c r="K148" s="5" t="n">
         <v>2.29</v>
       </c>
       <c r="L148" s="1" t="n">
@@ -7348,22 +7343,22 @@
       <c r="E149" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="F149" s="6" t="s">
+      <c r="F149" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="G149" s="9" t="s">
+      <c r="G149" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H149" s="15" t="s">
+      <c r="H149" s="14" t="s">
         <v>682</v>
       </c>
-      <c r="I149" s="6" t="s">
+      <c r="I149" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J149" s="6" t="n">
+      <c r="J149" s="5" t="n">
         <v>1609187</v>
       </c>
-      <c r="K149" s="6" t="n">
+      <c r="K149" s="5" t="n">
         <v>3.96</v>
       </c>
       <c r="L149" s="1" t="n">
@@ -7387,22 +7382,22 @@
       <c r="E150" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="F150" s="8" t="s">
+      <c r="F150" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="G150" s="9" t="s">
+      <c r="G150" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H150" s="8" t="s">
+      <c r="H150" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="I150" s="8" t="s">
+      <c r="I150" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J150" s="8" t="n">
+      <c r="J150" s="7" t="n">
         <v>1778211</v>
       </c>
-      <c r="K150" s="8" t="n">
+      <c r="K150" s="7" t="n">
         <v>2.23</v>
       </c>
       <c r="L150" s="1" t="n">
@@ -7426,22 +7421,22 @@
       <c r="E151" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="F151" s="8" t="s">
+      <c r="F151" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="G151" s="9" t="s">
+      <c r="G151" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H151" s="8" t="s">
+      <c r="H151" s="7" t="s">
         <v>694</v>
       </c>
-      <c r="I151" s="8" t="s">
+      <c r="I151" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J151" s="8" t="n">
+      <c r="J151" s="7" t="n">
         <v>1578449</v>
       </c>
-      <c r="K151" s="8" t="n">
+      <c r="K151" s="7" t="n">
         <v>0.639</v>
       </c>
       <c r="L151" s="1" t="n">
@@ -7465,22 +7460,22 @@
       <c r="E152" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="F152" s="8" t="s">
+      <c r="F152" s="7" t="s">
         <v>698</v>
       </c>
-      <c r="G152" s="9" t="s">
+      <c r="G152" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H152" s="8" t="s">
+      <c r="H152" s="7" t="s">
         <v>699</v>
       </c>
-      <c r="I152" s="8" t="s">
+      <c r="I152" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J152" s="8" t="n">
+      <c r="J152" s="7" t="n">
         <v>1234674</v>
       </c>
-      <c r="K152" s="8" t="n">
+      <c r="K152" s="7" t="n">
         <v>0.335</v>
       </c>
       <c r="L152" s="1" t="n">
@@ -7504,22 +7499,22 @@
       <c r="E153" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="F153" s="8" t="s">
+      <c r="F153" s="7" t="s">
         <v>704</v>
       </c>
-      <c r="G153" s="9" t="s">
+      <c r="G153" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H153" s="8" t="s">
+      <c r="H153" s="7" t="s">
         <v>705</v>
       </c>
-      <c r="I153" s="8" t="s">
+      <c r="I153" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J153" s="6" t="s">
+      <c r="J153" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="K153" s="8" t="n">
+      <c r="K153" s="7" t="n">
         <v>2.385</v>
       </c>
       <c r="L153" s="1" t="n">
@@ -7543,22 +7538,22 @@
       <c r="E154" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="F154" s="8" t="s">
+      <c r="F154" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="G154" s="9" t="s">
+      <c r="G154" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H154" s="8" t="s">
+      <c r="H154" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="I154" s="8" t="s">
+      <c r="I154" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J154" s="8" t="n">
+      <c r="J154" s="7" t="n">
         <v>2434896</v>
       </c>
-      <c r="K154" s="8" t="n">
+      <c r="K154" s="7" t="n">
         <v>0.719</v>
       </c>
       <c r="L154" s="1" t="n">
@@ -7582,22 +7577,22 @@
       <c r="E155" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="F155" s="8" t="s">
+      <c r="F155" s="7" t="s">
         <v>715</v>
       </c>
-      <c r="G155" s="9" t="s">
+      <c r="G155" s="8" t="s">
         <v>716</v>
       </c>
-      <c r="H155" s="8" t="s">
+      <c r="H155" s="7" t="s">
         <v>717</v>
       </c>
-      <c r="I155" s="8" t="s">
+      <c r="I155" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J155" s="8" t="s">
+      <c r="J155" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="K155" s="8" t="n">
+      <c r="K155" s="7" t="n">
         <v>2.23</v>
       </c>
       <c r="L155" s="1" t="n">
@@ -7621,22 +7616,22 @@
       <c r="E156" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="F156" s="8" t="s">
+      <c r="F156" s="7" t="s">
         <v>723</v>
       </c>
-      <c r="G156" s="9" t="s">
+      <c r="G156" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H156" s="8" t="s">
+      <c r="H156" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="I156" s="8" t="s">
+      <c r="I156" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J156" s="8" t="n">
+      <c r="J156" s="7" t="n">
         <v>2806158</v>
       </c>
-      <c r="K156" s="8" t="n">
+      <c r="K156" s="7" t="n">
         <v>1.5</v>
       </c>
       <c r="L156" s="1" t="n">
@@ -7660,22 +7655,22 @@
       <c r="E157" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="F157" s="8" t="s">
+      <c r="F157" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="G157" s="9" t="s">
+      <c r="G157" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="H157" s="8" t="s">
+      <c r="H157" s="7" t="s">
         <v>726</v>
       </c>
-      <c r="I157" s="8" t="s">
+      <c r="I157" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J157" s="8" t="n">
+      <c r="J157" s="7" t="n">
         <v>2400812</v>
       </c>
-      <c r="K157" s="8" t="n">
+      <c r="K157" s="7" t="n">
         <v>2.82</v>
       </c>
       <c r="L157" s="1" t="n">
@@ -7699,22 +7694,22 @@
       <c r="E158" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="F158" s="8" t="s">
+      <c r="F158" s="7" t="s">
         <v>735</v>
       </c>
-      <c r="G158" s="9" t="s">
+      <c r="G158" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H158" s="8" t="s">
+      <c r="H158" s="7" t="s">
         <v>736</v>
       </c>
-      <c r="I158" s="8" t="s">
+      <c r="I158" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J158" s="8" t="n">
+      <c r="J158" s="7" t="n">
         <v>2335695</v>
       </c>
-      <c r="K158" s="8" t="n">
+      <c r="K158" s="7" t="n">
         <v>4.41</v>
       </c>
       <c r="L158" s="1" t="n">
@@ -7738,22 +7733,22 @@
       <c r="E159" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="F159" s="8" t="s">
+      <c r="F159" s="7" t="s">
         <v>740</v>
       </c>
-      <c r="G159" s="9" t="s">
+      <c r="G159" s="8" t="s">
         <v>741</v>
       </c>
-      <c r="H159" s="8" t="s">
+      <c r="H159" s="7" t="s">
         <v>742</v>
       </c>
-      <c r="I159" s="8" t="s">
+      <c r="I159" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="J159" s="12" t="s">
+      <c r="J159" s="11" t="s">
         <v>743</v>
       </c>
-      <c r="K159" s="8" t="n">
+      <c r="K159" s="7" t="n">
         <v>0.21</v>
       </c>
       <c r="L159" s="1" t="n">
@@ -7777,22 +7772,22 @@
       <c r="E160" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="F160" s="16" t="s">
+      <c r="F160" s="15" t="s">
         <v>748</v>
       </c>
-      <c r="G160" s="9" t="s">
+      <c r="G160" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="H160" s="16" t="s">
+      <c r="H160" s="15" t="s">
         <v>745</v>
       </c>
-      <c r="I160" s="8" t="s">
+      <c r="I160" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J160" s="8" t="n">
+      <c r="J160" s="7" t="n">
         <v>2577278</v>
       </c>
-      <c r="K160" s="8" t="n">
+      <c r="K160" s="7" t="n">
         <v>1.27</v>
       </c>
       <c r="L160" s="1" t="n">
@@ -7816,22 +7811,22 @@
       <c r="E161" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="F161" s="16" t="s">
+      <c r="F161" s="15" t="s">
         <v>754</v>
       </c>
-      <c r="G161" s="9" t="s">
+      <c r="G161" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="H161" s="16" t="s">
+      <c r="H161" s="15" t="s">
         <v>755</v>
       </c>
-      <c r="I161" s="8" t="s">
+      <c r="I161" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="J161" s="8" t="s">
+      <c r="J161" s="7" t="s">
         <v>756</v>
       </c>
-      <c r="K161" s="8" t="n">
+      <c r="K161" s="7" t="n">
         <v>4.85</v>
       </c>
       <c r="L161" s="1" t="n">
@@ -7855,22 +7850,22 @@
       <c r="E162" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="F162" s="6" t="s">
+      <c r="F162" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="G162" s="9" t="s">
+      <c r="G162" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="H162" s="15" t="s">
+      <c r="H162" s="14" t="s">
         <v>761</v>
       </c>
-      <c r="I162" s="6" t="s">
+      <c r="I162" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J162" s="6" t="n">
+      <c r="J162" s="5" t="n">
         <v>2341651</v>
       </c>
-      <c r="K162" s="6" t="n">
+      <c r="K162" s="5" t="n">
         <v>0.448</v>
       </c>
       <c r="L162" s="1" t="n">
@@ -7894,22 +7889,22 @@
       <c r="E163" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="F163" s="16" t="s">
+      <c r="F163" s="15" t="s">
         <v>766</v>
       </c>
-      <c r="G163" s="9" t="s">
+      <c r="G163" s="8" t="s">
         <v>665</v>
       </c>
-      <c r="H163" s="8" t="s">
+      <c r="H163" s="7" t="s">
         <v>767</v>
       </c>
-      <c r="I163" s="8" t="s">
+      <c r="I163" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J163" s="8" t="n">
+      <c r="J163" s="7" t="n">
         <v>2517399</v>
       </c>
-      <c r="K163" s="13" t="n">
+      <c r="K163" s="12" t="n">
         <v>4.92</v>
       </c>
       <c r="L163" s="1" t="n">
@@ -7933,22 +7928,22 @@
       <c r="E164" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="F164" s="6" t="s">
+      <c r="F164" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="G164" s="9" t="s">
+      <c r="G164" s="8" t="s">
         <v>773</v>
       </c>
-      <c r="H164" s="15" t="s">
+      <c r="H164" s="14" t="s">
         <v>774</v>
       </c>
-      <c r="I164" s="6" t="s">
+      <c r="I164" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J164" s="6" t="n">
+      <c r="J164" s="5" t="n">
         <v>2508533</v>
       </c>
-      <c r="K164" s="6" t="n">
+      <c r="K164" s="5" t="n">
         <v>0.63</v>
       </c>
       <c r="L164" s="1" t="n">
@@ -7972,22 +7967,22 @@
       <c r="E165" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="F165" s="6" t="s">
+      <c r="F165" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="G165" s="9" t="s">
+      <c r="G165" s="8" t="s">
         <v>780</v>
       </c>
-      <c r="H165" s="6" t="s">
+      <c r="H165" s="5" t="s">
         <v>781</v>
       </c>
-      <c r="I165" s="6" t="s">
+      <c r="I165" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J165" s="6" t="n">
+      <c r="J165" s="5" t="n">
         <v>2101339</v>
       </c>
-      <c r="K165" s="6" t="n">
+      <c r="K165" s="5" t="n">
         <v>0.608</v>
       </c>
       <c r="L165" s="1" t="n">
@@ -8011,22 +8006,22 @@
       <c r="E166" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="F166" s="6" t="s">
+      <c r="F166" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="G166" s="9" t="s">
+      <c r="G166" s="8" t="s">
         <v>787</v>
       </c>
-      <c r="H166" s="15" t="s">
+      <c r="H166" s="14" t="s">
         <v>788</v>
       </c>
-      <c r="I166" s="6" t="s">
+      <c r="I166" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J166" s="6" t="n">
+      <c r="J166" s="5" t="n">
         <v>2061722</v>
       </c>
-      <c r="K166" s="6" t="n">
+      <c r="K166" s="5" t="n">
         <v>0.693</v>
       </c>
       <c r="L166" s="1" t="n">
@@ -8050,22 +8045,22 @@
       <c r="E167" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="F167" s="6" t="s">
+      <c r="F167" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="G167" s="9" t="s">
+      <c r="G167" s="8" t="s">
         <v>793</v>
       </c>
-      <c r="H167" s="6" t="s">
+      <c r="H167" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="I167" s="6" t="s">
+      <c r="I167" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J167" s="6" t="n">
+      <c r="J167" s="5" t="n">
         <v>1712847</v>
       </c>
-      <c r="K167" s="6" t="n">
+      <c r="K167" s="5" t="n">
         <v>0.524</v>
       </c>
       <c r="L167" s="1" t="n">
@@ -8089,22 +8084,22 @@
       <c r="E168" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="F168" s="6" t="s">
+      <c r="F168" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="G168" s="9" t="s">
+      <c r="G168" s="8" t="s">
         <v>787</v>
       </c>
-      <c r="H168" s="15" t="s">
+      <c r="H168" s="14" t="s">
         <v>800</v>
       </c>
-      <c r="I168" s="6" t="s">
+      <c r="I168" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J168" s="6" t="s">
+      <c r="J168" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="K168" s="6" t="n">
+      <c r="K168" s="5" t="n">
         <v>0.379</v>
       </c>
       <c r="L168" s="1" t="n">
@@ -8122,26 +8117,26 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="23" t="s">
+      <c r="A177" s="21" t="s">
         <v>803</v>
       </c>
-      <c r="B177" s="24" t="s">
+      <c r="B177" s="22" t="s">
         <v>804</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="24" t="s">
+      <c r="A178" s="22" t="s">
         <v>805</v>
       </c>
-      <c r="B178" s="24" t="s">
+      <c r="B178" s="22" t="s">
         <v>806</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="24" t="s">
+      <c r="A179" s="22" t="s">
         <v>807</v>
       </c>
-      <c r="B179" s="24" t="s">
+      <c r="B179" s="22" t="s">
         <v>808</v>
       </c>
     </row>

</xml_diff>